<commit_message>
Update CRT bot with detailed logging and cent account compatibility improvements
</commit_message>
<xml_diff>
--- a/trade_journal.xlsx
+++ b/trade_journal.xlsx
@@ -2,39 +2,378 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="22400" windowHeight="10120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -42,15 +381,305 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -403,7 +1032,6 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -413,13 +1041,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="13.6363636363636" customWidth="1" min="1" max="1"/>
+    <col width="27.3636363636364" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -525,10 +1157,10 @@
         <v>0.01</v>
       </c>
       <c r="I2" t="n">
-        <v>32.29149115417174</v>
+        <v>32.2914911541717</v>
       </c>
       <c r="J2" t="n">
-        <v>84.01432181971954</v>
+        <v>84.0143218197195</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -573,10 +1205,10 @@
         <v>0.01</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9798343234875018</v>
+        <v>0.979834323487502</v>
       </c>
       <c r="J3" t="n">
-        <v>2.316124173709069</v>
+        <v>2.31612417370907</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -669,10 +1301,10 @@
         <v>0.01</v>
       </c>
       <c r="I5" t="n">
-        <v>2.685771989692617</v>
+        <v>2.68577198969262</v>
       </c>
       <c r="J5" t="n">
-        <v>3.797966432202392</v>
+        <v>3.79796643220239</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -717,10 +1349,10 @@
         <v>0.01</v>
       </c>
       <c r="I6" t="n">
-        <v>2.884899999999993</v>
+        <v>2.88489999999999</v>
       </c>
       <c r="J6" t="n">
-        <v>5.769849999999996</v>
+        <v>5.76985</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -765,10 +1397,10 @@
         <v>0.01</v>
       </c>
       <c r="I7" t="n">
-        <v>2.884899999999993</v>
+        <v>2.88489999999999</v>
       </c>
       <c r="J7" t="n">
-        <v>5.769849999999996</v>
+        <v>5.76985</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -813,10 +1445,10 @@
         <v>0.01</v>
       </c>
       <c r="I8" t="n">
-        <v>2.884899999999993</v>
+        <v>2.88489999999999</v>
       </c>
       <c r="J8" t="n">
-        <v>5.769849999999996</v>
+        <v>5.76985</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -861,10 +1493,10 @@
         <v>0.01</v>
       </c>
       <c r="I9" t="n">
-        <v>2.884899999999993</v>
+        <v>2.88489999999999</v>
       </c>
       <c r="J9" t="n">
-        <v>5.769849999999996</v>
+        <v>5.76985</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -909,10 +1541,10 @@
         <v>0.01</v>
       </c>
       <c r="I10" t="n">
-        <v>2.706549999999993</v>
+        <v>2.70654999999999</v>
       </c>
       <c r="J10" t="n">
-        <v>5.413099999999986</v>
+        <v>5.41309999999999</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -957,10 +1589,10 @@
         <v>0.01</v>
       </c>
       <c r="I11" t="n">
-        <v>2.706549999999993</v>
+        <v>2.70654999999999</v>
       </c>
       <c r="J11" t="n">
-        <v>5.413099999999986</v>
+        <v>5.41309999999999</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -1005,10 +1637,10 @@
         <v>0.01</v>
       </c>
       <c r="I12" t="n">
-        <v>2.779899999999998</v>
+        <v>2.7799</v>
       </c>
       <c r="J12" t="n">
-        <v>5.559799999999996</v>
+        <v>5.5598</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -1053,10 +1685,10 @@
         <v>0.01</v>
       </c>
       <c r="I13" t="n">
-        <v>2.779899999999998</v>
+        <v>2.7799</v>
       </c>
       <c r="J13" t="n">
-        <v>5.559799999999996</v>
+        <v>5.5598</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1101,10 +1733,10 @@
         <v>0.01</v>
       </c>
       <c r="I14" t="n">
-        <v>2.939200000000005</v>
+        <v>2.9392</v>
       </c>
       <c r="J14" t="n">
-        <v>5.878400000000011</v>
+        <v>5.87840000000001</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1149,10 +1781,10 @@
         <v>0.01</v>
       </c>
       <c r="I15" t="n">
-        <v>2.939200000000005</v>
+        <v>2.9392</v>
       </c>
       <c r="J15" t="n">
-        <v>5.878400000000011</v>
+        <v>5.87840000000001</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1293,10 +1925,10 @@
         <v>0.01</v>
       </c>
       <c r="I18" t="n">
-        <v>2.034933333333326</v>
+        <v>2.03493333333333</v>
       </c>
       <c r="J18" t="n">
-        <v>4.069866666666682</v>
+        <v>4.06986666666668</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -1341,19 +1973,1270 @@
         <v>0.01</v>
       </c>
       <c r="I19" t="n">
-        <v>2.034933333333326</v>
+        <v>2.03493333333333</v>
       </c>
       <c r="J19" t="n">
-        <v>4.069866666666682</v>
+        <v>4.06986666666668</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
           <t>OPEN</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1993799578</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-07-31 16:16:16+00:00</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>3291.687</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3306.687</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3260.174</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2.10086666666666</v>
+      </c>
+      <c r="J20" t="n">
+        <v>4.2018</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1993799609</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-07-31 16:16:16+00:00</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>3291.687</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3306.687</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3228.66</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2.10086666666666</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4.2018</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2001158247</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2025-08-01 18:30:47+00:00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>3348.732</v>
+      </c>
+      <c r="F22" t="n">
+        <v>3363.732</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3316.354</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I22" t="n">
+        <v>2.15853333333334</v>
+      </c>
+      <c r="J22" t="n">
+        <v>4.31713333333334</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2001158255</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-08-01 18:30:47+00:00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>3348.732</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3363.732</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3283.975</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I23" t="n">
+        <v>2.15853333333334</v>
+      </c>
+      <c r="J23" t="n">
+        <v>4.31713333333334</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2015014537</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-08-05 10:28:20+00:00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>3357.42</v>
+      </c>
+      <c r="F24" t="n">
+        <v>3342.42</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3390.605</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I24" t="n">
+        <v>2.212333333333329</v>
+      </c>
+      <c r="J24" t="n">
+        <v>4.424666666666659</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2015014585</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-08-05 10:28:20+00:00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>3357.42</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3342.42</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3423.79</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I25" t="n">
+        <v>2.212333333333329</v>
+      </c>
+      <c r="J25" t="n">
+        <v>4.424666666666659</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2063297341</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-08-13 18:43:24+00:00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>3353.098</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3368.098</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3324.446</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1.910133333333336</v>
+      </c>
+      <c r="J26" t="n">
+        <v>3.820266666666673</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2063297349</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-08-13 18:43:24+00:00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>3353.098</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3368.098</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3295.794</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1.910133333333336</v>
+      </c>
+      <c r="J27" t="n">
+        <v>3.820266666666673</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2085238351</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-08-18 18:18:25+00:00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>3332.975</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3347.975</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3309.968</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1.533800000000004</v>
+      </c>
+      <c r="J28" t="n">
+        <v>3.067533333333328</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2085238355</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-08-18 18:18:25+00:00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>3332.975</v>
+      </c>
+      <c r="F29" t="n">
+        <v>3347.975</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3286.962</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1.533800000000004</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3.067533333333328</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2097723030</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-08-20 19:00:48+00:00</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>3345.376</v>
+      </c>
+      <c r="F30" t="n">
+        <v>3360.376</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3321.198</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1.611866666666689</v>
+      </c>
+      <c r="J30" t="n">
+        <v>3.223666666666668</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>2097723047</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-08-20 19:00:48+00:00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>3345.376</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3360.376</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3297.021</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1.611866666666689</v>
+      </c>
+      <c r="J31" t="n">
+        <v>3.223666666666668</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>2114291240</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-08-25 01:00:49+00:00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>3366.258</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3351.258</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3387.963</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1.447000000000025</v>
+      </c>
+      <c r="J32" t="n">
+        <v>2.893933333333341</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>2114291283</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-08-25 01:00:49+00:00</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>3366.258</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3351.258</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3409.667</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1.447000000000025</v>
+      </c>
+      <c r="J33" t="n">
+        <v>2.893933333333341</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>2128946321</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-08-27 01:00:13+00:00</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>3389.285</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3374.285</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3411.174</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1.459266666666675</v>
+      </c>
+      <c r="J34" t="n">
+        <v>2.9186</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2128946353</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2025-08-27 01:00:13+00:00</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>3389.285</v>
+      </c>
+      <c r="F35" t="n">
+        <v>3374.285</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3433.064</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1.459266666666675</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2.9186</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>2130047428</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2025-08-27 05:01:17+00:00</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>3375.357</v>
+      </c>
+      <c r="F36" t="n">
+        <v>3360.357</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3398.08</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1.514866666666664</v>
+      </c>
+      <c r="J36" t="n">
+        <v>3.029666666666678</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>2130047445</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-08-27 05:01:17+00:00</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>3375.357</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3360.357</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3420.802</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I37" t="n">
+        <v>1.514866666666664</v>
+      </c>
+      <c r="J37" t="n">
+        <v>3.029666666666678</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2145368978</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-08-29 01:00:07+00:00</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>3413.566</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3398.566</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3435.917</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1.490066666666674</v>
+      </c>
+      <c r="J38" t="n">
+        <v>2.980199999999998</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>2145369034</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025-08-29 01:00:07+00:00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>3413.566</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3398.566</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3458.269</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I39" t="n">
+        <v>1.490066666666674</v>
+      </c>
+      <c r="J39" t="n">
+        <v>2.980199999999998</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>2164048059</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025-09-02 01:00:43+00:00</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>3478.416</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3463.416</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3503.076</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1.64399999999999</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3.287999999999981</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>2164048128</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025-09-02 01:00:43+00:00</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>3478.416</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3463.416</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3527.736</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I41" t="n">
+        <v>1.64399999999999</v>
+      </c>
+      <c r="J41" t="n">
+        <v>3.287999999999981</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>2172963575</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2025-09-03 01:00:39+00:00</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>3537.986</v>
+      </c>
+      <c r="F42" t="n">
+        <v>3522.986</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3565.442</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I42" t="n">
+        <v>1.830400000000009</v>
+      </c>
+      <c r="J42" t="n">
+        <v>3.660800000000017</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2172963668</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025-09-03 01:00:39+00:00</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>3537.986</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3522.986</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3592.898</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I43" t="n">
+        <v>1.830400000000009</v>
+      </c>
+      <c r="J43" t="n">
+        <v>3.660800000000017</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>CRT advanced TP2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>2188525266</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2025-09-05 01:00:38+00:00</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>3553.328</v>
+      </c>
+      <c r="F44" t="n">
+        <v>3538.328</v>
+      </c>
+      <c r="G44" t="n">
+        <v>3581.864</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I44" t="n">
+        <v>1.902400000000004</v>
+      </c>
+      <c r="J44" t="n">
+        <v>3.804800000000008</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>CRT advanced TP1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>2188525314</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2025-09-05 01:00:38+00:00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>XAUUSDm</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>3553.328</v>
+      </c>
+      <c r="F45" t="n">
+        <v>3538.328</v>
+      </c>
+      <c r="G45" t="n">
+        <v>3610.4</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I45" t="n">
+        <v>1.902400000000004</v>
+      </c>
+      <c r="J45" t="n">
+        <v>3.804800000000008</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>OPEN</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr">
         <is>
           <t>CRT advanced TP2</t>
         </is>

</xml_diff>